<commit_message>
Panel pcb addition and stencils.
</commit_message>
<xml_diff>
--- a/bom.xlsx
+++ b/bom.xlsx
@@ -76,9 +76,6 @@
     <t>Stencils(50pcs)</t>
   </si>
   <si>
-    <t>Part 50pcs</t>
-  </si>
-  <si>
     <t>CAN CONNECTOR</t>
   </si>
   <si>
@@ -95,6 +92,9 @@
   </si>
   <si>
     <t>drukowane.pl</t>
+  </si>
+  <si>
+    <t>Part (50pcs)</t>
   </si>
 </sst>
 </file>
@@ -421,7 +421,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -431,8 +431,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E18"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -446,7 +446,7 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="B1" t="s">
         <v>9</v>
@@ -562,7 +562,7 @@
     </row>
     <row r="8" spans="1:5">
       <c r="A8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
@@ -572,7 +572,7 @@
     </row>
     <row r="9" spans="1:5">
       <c r="A9" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
@@ -582,7 +582,7 @@
     </row>
     <row r="10" spans="1:5">
       <c r="A10" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
@@ -592,7 +592,7 @@
     </row>
     <row r="11" spans="1:5">
       <c r="A11" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
@@ -602,7 +602,7 @@
     </row>
     <row r="12" spans="1:5">
       <c r="A12" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
@@ -629,12 +629,12 @@
         <v>12</v>
       </c>
       <c r="C15" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="16" spans="1:5">
       <c r="C16" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="17" spans="1:4">
@@ -648,7 +648,7 @@
     <row r="18" spans="1:4">
       <c r="D18">
         <f>D13+C16+C17</f>
-        <v>24.629999999999995</v>
+        <v>23.629999999999995</v>
       </c>
     </row>
   </sheetData>

</xml_diff>